<commit_message>
add Nr cell for both annotators
</commit_message>
<xml_diff>
--- a/Selected_WSIs.xlsx
+++ b/Selected_WSIs.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dars\PhD\projects\intraoperative histology samples\publihsed_git_repo\CryoNuSeg\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43EACA38-DC5E-404C-BBB5-76329C766270}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="-270" windowWidth="27015" windowHeight="12465"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Current Candidates" sheetId="1" r:id="rId1"/>
@@ -18,12 +24,22 @@
     <sheet name="Adrenal Gland" sheetId="9" r:id="rId9"/>
     <sheet name="Lymph Nodes" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="350">
   <si>
     <t>URL</t>
   </si>
@@ -952,9 +968,6 @@
     <t>Testes</t>
   </si>
   <si>
-    <t>Nr Cells</t>
-  </si>
-  <si>
     <t>Larynx</t>
   </si>
   <si>
@@ -1079,13 +1092,19 @@
   </si>
   <si>
     <t>Medium: Low contrast, odd coloring</t>
+  </si>
+  <si>
+    <t>Nr Cells(bioinformatician)</t>
+  </si>
+  <si>
+    <t>Nr Cells(biologist)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1095,44 +1114,52 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <i/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="11">
@@ -1238,10 +1265,18 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1442,24 +1477,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:Y53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q33" sqref="Q33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="43" customWidth="1"/>
-    <col min="13" max="13" width="21.42578125" customWidth="1"/>
-    <col min="14" max="14" width="30.28515625" customWidth="1"/>
+    <col min="13" max="13" width="21.44140625" customWidth="1"/>
+    <col min="14" max="14" width="30.33203125" customWidth="1"/>
+    <col min="16" max="16" width="22.77734375" customWidth="1"/>
+    <col min="17" max="17" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="12.75">
+    <row r="1" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1505,14 +1542,17 @@
       <c r="O1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="18" t="s">
-        <v>306</v>
-      </c>
-      <c r="Q1" s="18" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" ht="12.75">
+      <c r="P1" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="R1" s="18" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>175</v>
       </c>
@@ -1561,11 +1601,14 @@
       <c r="P2">
         <v>134</v>
       </c>
-      <c r="Q2" s="4" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" ht="12.75">
+      <c r="Q2" s="4">
+        <v>85</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>183</v>
       </c>
@@ -1614,11 +1657,14 @@
       <c r="P3">
         <v>127</v>
       </c>
-      <c r="Q3" s="4" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" ht="12.75">
+      <c r="Q3">
+        <v>119</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>187</v>
       </c>
@@ -1667,16 +1713,19 @@
       <c r="P4">
         <v>131</v>
       </c>
-      <c r="Q4" s="4" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" ht="12.75">
+      <c r="Q4">
+        <v>134</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>26</v>
@@ -1688,7 +1737,7 @@
         <v>-25469</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G5" s="4">
         <v>8</v>
@@ -1706,10 +1755,10 @@
         <v>0.22650000000000001</v>
       </c>
       <c r="L5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="M5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="N5" s="4">
         <v>8820.6551999999992</v>
@@ -1720,16 +1769,19 @@
       <c r="P5" s="4">
         <v>267</v>
       </c>
-      <c r="Q5" s="4" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" ht="12.75">
+      <c r="Q5" s="4">
+        <v>220</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>29</v>
@@ -1741,7 +1793,7 @@
         <v>-27456</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G6" s="4">
         <v>8</v>
@@ -1759,10 +1811,10 @@
         <v>0.24679999999999999</v>
       </c>
       <c r="L6" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="M6" s="18" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="N6" s="4">
         <v>3995.3935000000001</v>
@@ -1773,8 +1825,11 @@
       <c r="P6" s="4">
         <v>280</v>
       </c>
-      <c r="Q6" s="4" t="s">
-        <v>324</v>
+      <c r="Q6" s="4">
+        <v>224</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>323</v>
       </c>
       <c r="T6" s="9"/>
       <c r="U6" s="9"/>
@@ -1783,12 +1838,12 @@
       <c r="X6" s="9"/>
       <c r="Y6" s="9"/>
     </row>
-    <row r="7" spans="1:25" ht="12.75">
+    <row r="7" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B7" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C7" t="s">
         <v>52</v>
@@ -1800,7 +1855,7 @@
         <v>-22442</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G7" s="4">
         <v>8</v>
@@ -1818,10 +1873,10 @@
         <v>0.24560000000000001</v>
       </c>
       <c r="L7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="M7" s="18" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="N7" s="4">
         <v>19627.148300000001</v>
@@ -1832,11 +1887,14 @@
       <c r="P7" s="4">
         <v>218</v>
       </c>
-      <c r="Q7" s="4" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" ht="12.75">
+      <c r="Q7" s="4">
+        <v>178</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>191</v>
       </c>
@@ -1885,11 +1943,14 @@
       <c r="P8">
         <v>417</v>
       </c>
-      <c r="Q8" s="4" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" ht="12.75">
+      <c r="Q8" s="4">
+        <v>261</v>
+      </c>
+      <c r="R8" s="4" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>198</v>
       </c>
@@ -1938,11 +1999,14 @@
       <c r="P9">
         <v>433</v>
       </c>
-      <c r="Q9" s="4" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" ht="12.75">
+      <c r="Q9" s="4">
+        <v>428</v>
+      </c>
+      <c r="R9" s="4" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>115</v>
       </c>
@@ -1991,11 +2055,14 @@
       <c r="P10">
         <v>503</v>
       </c>
-      <c r="Q10" s="4" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" ht="12.75">
+      <c r="Q10" s="4">
+        <v>515</v>
+      </c>
+      <c r="R10" s="4" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>125</v>
       </c>
@@ -2044,11 +2111,14 @@
       <c r="P11">
         <v>624</v>
       </c>
-      <c r="Q11" s="4" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" ht="12.75">
+      <c r="Q11" s="4">
+        <v>573</v>
+      </c>
+      <c r="R11" s="4" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>135</v>
       </c>
@@ -2097,12 +2167,15 @@
       <c r="P12">
         <v>419</v>
       </c>
-      <c r="Q12" s="4" t="s">
-        <v>331</v>
+      <c r="Q12" s="4">
+        <v>380</v>
+      </c>
+      <c r="R12" s="4" t="s">
+        <v>330</v>
       </c>
       <c r="T12" s="4"/>
     </row>
-    <row r="13" spans="1:25" ht="12.75">
+    <row r="13" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>141</v>
       </c>
@@ -2151,11 +2224,14 @@
       <c r="P13">
         <v>311</v>
       </c>
-      <c r="Q13" s="4" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" ht="12.75">
+      <c r="Q13" s="4">
+        <v>321</v>
+      </c>
+      <c r="R13" s="4" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>88</v>
       </c>
@@ -2204,11 +2280,14 @@
       <c r="P14">
         <v>239</v>
       </c>
-      <c r="Q14" s="4" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" ht="12.75">
+      <c r="Q14" s="4">
+        <v>136</v>
+      </c>
+      <c r="R14" s="4" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>96</v>
       </c>
@@ -2257,11 +2336,14 @@
       <c r="P15">
         <v>226</v>
       </c>
-      <c r="Q15" s="4" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" ht="12.75">
+      <c r="Q15" s="4">
+        <v>221</v>
+      </c>
+      <c r="R15" s="4" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>103</v>
       </c>
@@ -2310,11 +2392,14 @@
       <c r="P16">
         <v>158</v>
       </c>
-      <c r="Q16" s="4" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" ht="12.75">
+      <c r="Q16" s="4">
+        <v>113</v>
+      </c>
+      <c r="R16" s="4" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>108</v>
       </c>
@@ -2363,11 +2448,14 @@
       <c r="P17">
         <v>207</v>
       </c>
-      <c r="Q17" s="4" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" ht="12.75">
+      <c r="Q17" s="4">
+        <v>168</v>
+      </c>
+      <c r="R17" s="4" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>113</v>
       </c>
@@ -2416,11 +2504,14 @@
       <c r="P18">
         <v>265</v>
       </c>
-      <c r="Q18" s="4" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" ht="12.75">
+      <c r="Q18" s="4">
+        <v>177</v>
+      </c>
+      <c r="R18" s="4" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>118</v>
       </c>
@@ -2469,11 +2560,14 @@
       <c r="P19">
         <v>166</v>
       </c>
-      <c r="Q19" s="4" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" ht="15.75" customHeight="1">
+      <c r="Q19" s="4">
+        <v>152</v>
+      </c>
+      <c r="R19" s="4" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>60</v>
       </c>
@@ -2522,11 +2616,14 @@
       <c r="P20">
         <v>138</v>
       </c>
-      <c r="Q20" s="4" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" ht="15.75" customHeight="1">
+      <c r="Q20" s="4">
+        <v>144</v>
+      </c>
+      <c r="R20" s="4" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>70</v>
       </c>
@@ -2575,11 +2672,14 @@
       <c r="P21">
         <v>159</v>
       </c>
-      <c r="Q21" s="4" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" ht="15.75" customHeight="1">
+      <c r="Q21" s="4">
+        <v>126</v>
+      </c>
+      <c r="R21" s="4" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>81</v>
       </c>
@@ -2628,11 +2728,14 @@
       <c r="P22">
         <v>210</v>
       </c>
-      <c r="Q22" s="4" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" ht="12.75">
+      <c r="Q22" s="4">
+        <v>187</v>
+      </c>
+      <c r="R22" s="4" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>300</v>
       </c>
@@ -2672,11 +2775,14 @@
       <c r="P23">
         <v>279</v>
       </c>
-      <c r="Q23" s="4" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" ht="12.75">
+      <c r="Q23" s="4">
+        <v>274</v>
+      </c>
+      <c r="R23" s="4" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
         <v>301</v>
       </c>
@@ -2725,11 +2831,14 @@
       <c r="P24">
         <v>204</v>
       </c>
-      <c r="Q24" s="4" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" ht="12.75">
+      <c r="Q24" s="4">
+        <v>249</v>
+      </c>
+      <c r="R24" s="4" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>302</v>
       </c>
@@ -2778,11 +2887,14 @@
       <c r="P25">
         <v>204</v>
       </c>
-      <c r="Q25" s="4" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" ht="12.75">
+      <c r="Q25" s="4">
+        <v>229</v>
+      </c>
+      <c r="R25" s="4" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>149</v>
       </c>
@@ -2831,11 +2943,14 @@
       <c r="P26">
         <v>570</v>
       </c>
-      <c r="Q26" s="4" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" ht="12.75">
+      <c r="Q26" s="4">
+        <v>638</v>
+      </c>
+      <c r="R26" s="4" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>160</v>
       </c>
@@ -2884,11 +2999,14 @@
       <c r="P27">
         <v>587</v>
       </c>
-      <c r="Q27" s="4" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" ht="12.75">
+      <c r="Q27" s="4">
+        <v>597</v>
+      </c>
+      <c r="R27" s="4" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>169</v>
       </c>
@@ -2937,11 +3055,14 @@
       <c r="P28">
         <v>326</v>
       </c>
-      <c r="Q28" s="4" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" ht="15.75" customHeight="1">
+      <c r="Q28" s="4">
+        <v>286</v>
+      </c>
+      <c r="R28" s="4" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>18</v>
       </c>
@@ -2990,11 +3111,14 @@
       <c r="P29">
         <v>110</v>
       </c>
-      <c r="Q29" s="4" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" ht="15.75" customHeight="1">
+      <c r="Q29" s="4">
+        <v>117</v>
+      </c>
+      <c r="R29" s="4" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>45</v>
       </c>
@@ -3043,11 +3167,14 @@
       <c r="P30">
         <v>156</v>
       </c>
-      <c r="Q30" s="4" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" ht="15.75" customHeight="1">
+      <c r="Q30" s="4">
+        <v>158</v>
+      </c>
+      <c r="R30" s="4" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>57</v>
       </c>
@@ -3096,22 +3223,29 @@
       <c r="P31">
         <v>183</v>
       </c>
-      <c r="Q31" s="4" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" ht="15.75" customHeight="1">
+      <c r="Q31" s="4">
+        <v>186</v>
+      </c>
+      <c r="R31" s="4" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="P32">
         <f>SUM(P2:P31)</f>
         <v>8251</v>
       </c>
-    </row>
-    <row r="50" spans="7:10" ht="12.75">
+      <c r="Q32">
+        <f>SUM(Q2:Q31)</f>
+        <v>7596</v>
+      </c>
+    </row>
+    <row r="50" spans="7:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G50" s="4" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="52" spans="7:10" ht="12.75">
+    <row r="52" spans="7:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G52" s="6" t="s">
         <v>204</v>
       </c>
@@ -3125,7 +3259,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="53" spans="7:10" ht="12.75">
+    <row r="53" spans="7:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G53" s="8" t="s">
         <v>207</v>
       </c>
@@ -3137,40 +3271,40 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:Q31">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q31">
     <sortCondition ref="M2:M31"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="A29" r:id="rId1"/>
-    <hyperlink ref="A30" r:id="rId2"/>
-    <hyperlink ref="A31" r:id="rId3"/>
-    <hyperlink ref="A20" r:id="rId4"/>
-    <hyperlink ref="A21" r:id="rId5"/>
-    <hyperlink ref="A22" r:id="rId6"/>
-    <hyperlink ref="A14" r:id="rId7"/>
-    <hyperlink ref="A15" r:id="rId8"/>
-    <hyperlink ref="A16" r:id="rId9"/>
-    <hyperlink ref="A17" r:id="rId10"/>
-    <hyperlink ref="A18" r:id="rId11"/>
-    <hyperlink ref="A19" r:id="rId12"/>
-    <hyperlink ref="A11" r:id="rId13"/>
-    <hyperlink ref="A12" r:id="rId14"/>
-    <hyperlink ref="A13" r:id="rId15"/>
-    <hyperlink ref="A26" r:id="rId16"/>
-    <hyperlink ref="A27" r:id="rId17"/>
-    <hyperlink ref="A28" r:id="rId18"/>
-    <hyperlink ref="A2" r:id="rId19"/>
-    <hyperlink ref="A3" r:id="rId20"/>
-    <hyperlink ref="A4" r:id="rId21"/>
-    <hyperlink ref="A8" r:id="rId22"/>
-    <hyperlink ref="A9" r:id="rId23"/>
-    <hyperlink ref="A10" r:id="rId24"/>
-    <hyperlink ref="A23" r:id="rId25"/>
-    <hyperlink ref="A5" r:id="rId26"/>
-    <hyperlink ref="A6" r:id="rId27"/>
-    <hyperlink ref="A7" r:id="rId28"/>
-    <hyperlink ref="A24" r:id="rId29"/>
-    <hyperlink ref="A25" r:id="rId30"/>
+    <hyperlink ref="A29" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A30" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A31" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="A20" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="A21" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="A22" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="A14" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="A15" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="A16" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="A17" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="A18" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="A19" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="A11" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="A12" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="A13" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="A26" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="A27" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="A28" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="A2" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="A3" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="A4" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="A8" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="A9" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="A10" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="A23" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="A5" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="A6" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="A7" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="A24" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="A25" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId31"/>
@@ -3178,7 +3312,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -3186,16 +3320,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="12.75">
+    <row r="1" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
@@ -3233,7 +3367,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="12.75">
+    <row r="2" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>267</v>
       </c>
@@ -3274,7 +3408,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="12.75">
+    <row r="3" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>271</v>
       </c>
@@ -3315,7 +3449,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="12.75">
+    <row r="4" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>274</v>
       </c>
@@ -3356,7 +3490,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="12.75">
+    <row r="5" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>191</v>
       </c>
@@ -3397,7 +3531,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="12.75">
+    <row r="6" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>198</v>
       </c>
@@ -3438,7 +3572,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="12.75">
+    <row r="7" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>278</v>
       </c>
@@ -3479,7 +3613,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="12.75">
+    <row r="8" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>282</v>
       </c>
@@ -3520,7 +3654,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15" customHeight="1">
+    <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>285</v>
       </c>
@@ -3561,7 +3695,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="12.75">
+    <row r="10" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>287</v>
       </c>
@@ -3602,7 +3736,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="12.75">
+    <row r="11" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>289</v>
       </c>
@@ -3643,7 +3777,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="12.75">
+    <row r="12" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>291</v>
       </c>
@@ -3684,34 +3818,34 @@
         <v>196</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="12.75">
+    <row r="13" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
     </row>
-    <row r="15" spans="1:13" ht="12.75">
+    <row r="15" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>293</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
-    <hyperlink ref="A8" r:id="rId7"/>
-    <hyperlink ref="A9" r:id="rId8"/>
-    <hyperlink ref="A10" r:id="rId9"/>
-    <hyperlink ref="A11" r:id="rId10"/>
-    <hyperlink ref="A12" r:id="rId11"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{00000000-0004-0000-0900-000002000000}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{00000000-0004-0000-0900-000003000000}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{00000000-0004-0000-0900-000004000000}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{00000000-0004-0000-0900-000005000000}"/>
+    <hyperlink ref="A8" r:id="rId7" xr:uid="{00000000-0004-0000-0900-000006000000}"/>
+    <hyperlink ref="A9" r:id="rId8" xr:uid="{00000000-0004-0000-0900-000007000000}"/>
+    <hyperlink ref="A10" r:id="rId9" xr:uid="{00000000-0004-0000-0900-000008000000}"/>
+    <hyperlink ref="A11" r:id="rId10" xr:uid="{00000000-0004-0000-0900-000009000000}"/>
+    <hyperlink ref="A12" r:id="rId11" xr:uid="{00000000-0004-0000-0900-00000A000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -3719,12 +3853,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="12.75">
+    <row r="1" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
@@ -3762,7 +3896,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="12.75">
+    <row r="2" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>16</v>
       </c>
@@ -3797,7 +3931,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="12.75">
+    <row r="3" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
@@ -3832,7 +3966,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="12.75">
+    <row r="4" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>28</v>
       </c>
@@ -3867,7 +4001,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="12.75">
+    <row r="5" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>30</v>
       </c>
@@ -3902,7 +4036,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="12.75">
+    <row r="6" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>31</v>
       </c>
@@ -3937,7 +4071,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="12.75">
+    <row r="7" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>34</v>
       </c>
@@ -3972,7 +4106,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="12.75">
+    <row r="8" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>38</v>
       </c>
@@ -4007,7 +4141,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15" customHeight="1">
+    <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>42</v>
       </c>
@@ -4042,7 +4176,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="12.75">
+    <row r="10" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>46</v>
       </c>
@@ -4077,7 +4211,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="12.75">
+    <row r="11" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>48</v>
       </c>
@@ -4112,7 +4246,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="12.75">
+    <row r="12" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>49</v>
       </c>
@@ -4147,7 +4281,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="12.75">
+    <row r="13" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>50</v>
       </c>
@@ -4182,7 +4316,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="12.75">
+    <row r="14" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
         <v>53</v>
       </c>
@@ -4217,7 +4351,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="12.75">
+    <row r="15" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>56</v>
       </c>
@@ -4255,7 +4389,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="12.75">
+    <row r="16" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>62</v>
       </c>
@@ -4293,7 +4427,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="12.75">
+    <row r="17" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>71</v>
       </c>
@@ -4331,7 +4465,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="12.75">
+    <row r="18" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>80</v>
       </c>
@@ -4371,17 +4505,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A15" r:id="rId1"/>
-    <hyperlink ref="A16" r:id="rId2"/>
-    <hyperlink ref="A17" r:id="rId3"/>
-    <hyperlink ref="A18" r:id="rId4"/>
+    <hyperlink ref="A15" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="A16" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="A17" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="A18" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -4389,15 +4523,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" customWidth="1"/>
+    <col min="6" max="6" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="12.75">
+    <row r="1" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
@@ -4435,7 +4569,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="12.75">
+    <row r="2" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>19</v>
       </c>
@@ -4476,7 +4610,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="12.75">
+    <row r="3" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>45</v>
       </c>
@@ -4517,7 +4651,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="12.75">
+    <row r="4" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
@@ -4558,7 +4692,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="12.75">
+    <row r="5" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>57</v>
       </c>
@@ -4599,7 +4733,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="12.75">
+    <row r="6" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>68</v>
       </c>
@@ -4640,7 +4774,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="12.75">
+    <row r="7" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>79</v>
       </c>
@@ -4681,7 +4815,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="12.75">
+    <row r="8" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>86</v>
       </c>
@@ -4722,7 +4856,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15" customHeight="1">
+    <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>93</v>
       </c>
@@ -4763,7 +4897,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="12.75">
+    <row r="10" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>98</v>
       </c>
@@ -4804,33 +4938,33 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="12.75">
+    <row r="11" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:13" ht="12.75">
+    <row r="12" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:13" ht="12.75">
+    <row r="13" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
-    <hyperlink ref="A8" r:id="rId7"/>
-    <hyperlink ref="A9" r:id="rId8"/>
-    <hyperlink ref="A10" r:id="rId9"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="A8" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="A9" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="A10" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -4838,15 +4972,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" customWidth="1"/>
+    <col min="6" max="6" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="12.75">
+    <row r="1" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
@@ -4884,7 +5018,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="12.75">
+    <row r="2" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>115</v>
       </c>
@@ -4925,7 +5059,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="12.75">
+    <row r="3" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>122</v>
       </c>
@@ -4966,7 +5100,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="12.75">
+    <row r="4" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>132</v>
       </c>
@@ -5007,7 +5141,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="12.75">
+    <row r="5" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>60</v>
       </c>
@@ -5048,7 +5182,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="12.75">
+    <row r="6" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>143</v>
       </c>
@@ -5089,7 +5223,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="12.75">
+    <row r="7" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>152</v>
       </c>
@@ -5130,7 +5264,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="12.75">
+    <row r="8" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>161</v>
       </c>
@@ -5171,7 +5305,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15" customHeight="1">
+    <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>70</v>
       </c>
@@ -5212,7 +5346,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="12.75">
+    <row r="10" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>176</v>
       </c>
@@ -5253,7 +5387,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="12.75">
+    <row r="11" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>81</v>
       </c>
@@ -5294,31 +5428,31 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="12.75">
+    <row r="12" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:13" ht="12.75">
+    <row r="13" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
-    <hyperlink ref="A8" r:id="rId7"/>
-    <hyperlink ref="A9" r:id="rId8"/>
-    <hyperlink ref="A10" r:id="rId9"/>
-    <hyperlink ref="A11" r:id="rId10"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
+    <hyperlink ref="A8" r:id="rId7" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
+    <hyperlink ref="A9" r:id="rId8" xr:uid="{00000000-0004-0000-0300-000007000000}"/>
+    <hyperlink ref="A10" r:id="rId9" xr:uid="{00000000-0004-0000-0300-000008000000}"/>
+    <hyperlink ref="A11" r:id="rId10" xr:uid="{00000000-0004-0000-0300-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -5326,16 +5460,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="12.75">
+    <row r="1" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
@@ -5373,7 +5507,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="12.75">
+    <row r="2" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>108</v>
       </c>
@@ -5414,7 +5548,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="12.75">
+    <row r="3" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>138</v>
       </c>
@@ -5455,7 +5589,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="12.75">
+    <row r="4" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>147</v>
       </c>
@@ -5496,7 +5630,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="12.75">
+    <row r="5" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>135</v>
       </c>
@@ -5537,7 +5671,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="12.75">
+    <row r="6" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>162</v>
       </c>
@@ -5578,7 +5712,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="12.75">
+    <row r="7" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>174</v>
       </c>
@@ -5619,7 +5753,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="12.75">
+    <row r="8" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>113</v>
       </c>
@@ -5660,7 +5794,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15" customHeight="1">
+    <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>188</v>
       </c>
@@ -5701,7 +5835,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="12.75">
+    <row r="10" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>141</v>
       </c>
@@ -5742,7 +5876,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="12.75">
+    <row r="11" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>125</v>
       </c>
@@ -5783,7 +5917,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="12.75">
+    <row r="12" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>118</v>
       </c>
@@ -5824,29 +5958,29 @@
         <v>111</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="12.75">
+    <row r="13" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
-    <hyperlink ref="A8" r:id="rId7"/>
-    <hyperlink ref="A9" r:id="rId8"/>
-    <hyperlink ref="A10" r:id="rId9"/>
-    <hyperlink ref="A11" r:id="rId10"/>
-    <hyperlink ref="A12" r:id="rId11"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
+    <hyperlink ref="A8" r:id="rId7" xr:uid="{00000000-0004-0000-0400-000006000000}"/>
+    <hyperlink ref="A9" r:id="rId8" xr:uid="{00000000-0004-0000-0400-000007000000}"/>
+    <hyperlink ref="A10" r:id="rId9" xr:uid="{00000000-0004-0000-0400-000008000000}"/>
+    <hyperlink ref="A11" r:id="rId10" xr:uid="{00000000-0004-0000-0400-000009000000}"/>
+    <hyperlink ref="A12" r:id="rId11" xr:uid="{00000000-0004-0000-0400-00000A000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -5854,15 +5988,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" customWidth="1"/>
+    <col min="6" max="6" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="12.75">
+    <row r="1" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
@@ -5900,7 +6034,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="12.75">
+    <row r="2" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>210</v>
       </c>
@@ -5941,7 +6075,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="12.75">
+    <row r="3" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>96</v>
       </c>
@@ -5982,7 +6116,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="12.75">
+    <row r="4" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>213</v>
       </c>
@@ -6023,7 +6157,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="12.75">
+    <row r="5" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>216</v>
       </c>
@@ -6064,7 +6198,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="12.75">
+    <row r="6" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>225</v>
       </c>
@@ -6105,7 +6239,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="12.75">
+    <row r="7" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>103</v>
       </c>
@@ -6146,7 +6280,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="12.75">
+    <row r="8" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>240</v>
       </c>
@@ -6187,7 +6321,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15" customHeight="1">
+    <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>88</v>
       </c>
@@ -6228,7 +6362,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="12.75">
+    <row r="10" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>247</v>
       </c>
@@ -6269,7 +6403,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="12.75">
+    <row r="11" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>251</v>
       </c>
@@ -6310,31 +6444,31 @@
         <v>101</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="12.75">
+    <row r="12" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:13" ht="12.75">
+    <row r="13" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
-    <hyperlink ref="A8" r:id="rId7"/>
-    <hyperlink ref="A9" r:id="rId8"/>
-    <hyperlink ref="A10" r:id="rId9"/>
-    <hyperlink ref="A11" r:id="rId10"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
+    <hyperlink ref="A8" r:id="rId7" xr:uid="{00000000-0004-0000-0500-000006000000}"/>
+    <hyperlink ref="A9" r:id="rId8" xr:uid="{00000000-0004-0000-0500-000007000000}"/>
+    <hyperlink ref="A10" r:id="rId9" xr:uid="{00000000-0004-0000-0500-000008000000}"/>
+    <hyperlink ref="A11" r:id="rId10" xr:uid="{00000000-0004-0000-0500-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -6342,16 +6476,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="12.75">
+    <row r="1" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
@@ -6389,7 +6523,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="12.75">
+    <row r="2" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>169</v>
       </c>
@@ -6430,7 +6564,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="12.75">
+    <row r="3" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>160</v>
       </c>
@@ -6471,7 +6605,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="12.75">
+    <row r="4" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>224</v>
       </c>
@@ -6512,7 +6646,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="12.75">
+    <row r="5" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>229</v>
       </c>
@@ -6553,7 +6687,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="12.75">
+    <row r="6" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>234</v>
       </c>
@@ -6594,7 +6728,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="12.75">
+    <row r="7" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>239</v>
       </c>
@@ -6635,7 +6769,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="12.75">
+    <row r="8" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>242</v>
       </c>
@@ -6676,7 +6810,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15" customHeight="1">
+    <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>245</v>
       </c>
@@ -6717,7 +6851,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="12.75">
+    <row r="10" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>149</v>
       </c>
@@ -6758,7 +6892,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="12.75">
+    <row r="11" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>248</v>
       </c>
@@ -6799,7 +6933,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="12.75">
+    <row r="12" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>252</v>
       </c>
@@ -6840,29 +6974,29 @@
         <v>255</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="12.75">
+    <row r="13" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
-    <hyperlink ref="A8" r:id="rId7"/>
-    <hyperlink ref="A9" r:id="rId8"/>
-    <hyperlink ref="A10" r:id="rId9"/>
-    <hyperlink ref="A11" r:id="rId10"/>
-    <hyperlink ref="A12" r:id="rId11"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{00000000-0004-0000-0600-000004000000}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{00000000-0004-0000-0600-000005000000}"/>
+    <hyperlink ref="A8" r:id="rId7" xr:uid="{00000000-0004-0000-0600-000006000000}"/>
+    <hyperlink ref="A9" r:id="rId8" xr:uid="{00000000-0004-0000-0600-000007000000}"/>
+    <hyperlink ref="A10" r:id="rId9" xr:uid="{00000000-0004-0000-0600-000008000000}"/>
+    <hyperlink ref="A11" r:id="rId10" xr:uid="{00000000-0004-0000-0600-000009000000}"/>
+    <hyperlink ref="A12" r:id="rId11" xr:uid="{00000000-0004-0000-0600-00000A000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -6870,16 +7004,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="12.75">
+    <row r="1" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
@@ -6917,7 +7051,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="12.75">
+    <row r="2" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>215</v>
       </c>
@@ -6958,7 +7092,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="12.75">
+    <row r="3" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>226</v>
       </c>
@@ -6999,7 +7133,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="12.75">
+    <row r="4" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>232</v>
       </c>
@@ -7040,47 +7174,47 @@
         <v>196</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="12.75">
+    <row r="5" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:13" ht="12.75">
+    <row r="6" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:13" ht="12.75">
+    <row r="7" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="12.75">
+    <row r="8" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:13" ht="15" customHeight="1">
+    <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:13" ht="12.75">
+    <row r="10" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:13" ht="12.75">
+    <row r="11" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:13" ht="12.75">
+    <row r="12" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:13" ht="12.75">
+    <row r="13" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -7088,16 +7222,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="12.75">
+    <row r="1" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
@@ -7135,7 +7269,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="12.75">
+    <row r="2" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>175</v>
       </c>
@@ -7176,7 +7310,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="12.75">
+    <row r="3" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>256</v>
       </c>
@@ -7217,7 +7351,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="12.75">
+    <row r="4" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>258</v>
       </c>
@@ -7258,7 +7392,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="12.75">
+    <row r="5" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>262</v>
       </c>
@@ -7299,7 +7433,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="12.75">
+    <row r="6" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>264</v>
       </c>
@@ -7340,7 +7474,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="12.75">
+    <row r="7" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>266</v>
       </c>
@@ -7381,7 +7515,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="12.75">
+    <row r="8" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>270</v>
       </c>
@@ -7422,7 +7556,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15" customHeight="1">
+    <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>275</v>
       </c>
@@ -7463,7 +7597,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="12.75">
+    <row r="10" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>183</v>
       </c>
@@ -7504,7 +7638,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="12.75">
+    <row r="11" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>279</v>
       </c>
@@ -7542,7 +7676,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="12.75">
+    <row r="12" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>280</v>
       </c>
@@ -7583,7 +7717,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="12.75">
+    <row r="13" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>187</v>
       </c>
@@ -7626,17 +7760,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
-    <hyperlink ref="A8" r:id="rId7"/>
-    <hyperlink ref="A9" r:id="rId8"/>
-    <hyperlink ref="A10" r:id="rId9"/>
-    <hyperlink ref="A12" r:id="rId10"/>
-    <hyperlink ref="A13" r:id="rId11"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{00000000-0004-0000-0800-000003000000}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{00000000-0004-0000-0800-000004000000}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{00000000-0004-0000-0800-000005000000}"/>
+    <hyperlink ref="A8" r:id="rId7" xr:uid="{00000000-0004-0000-0800-000006000000}"/>
+    <hyperlink ref="A9" r:id="rId8" xr:uid="{00000000-0004-0000-0800-000007000000}"/>
+    <hyperlink ref="A10" r:id="rId9" xr:uid="{00000000-0004-0000-0800-000008000000}"/>
+    <hyperlink ref="A12" r:id="rId10" xr:uid="{00000000-0004-0000-0800-000009000000}"/>
+    <hyperlink ref="A13" r:id="rId11" xr:uid="{00000000-0004-0000-0800-00000A000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add info second round mark-ups to excel file
</commit_message>
<xml_diff>
--- a/Selected_WSIs.xlsx
+++ b/Selected_WSIs.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dars\PhD\projects\intraoperative histology samples\publihsed_git_repo\CryoNuSeg\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08D2BC9B-4824-44BF-B639-BDD0BD897B9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Current Candidates" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -24,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="193">
   <si>
     <t>URL</t>
   </si>
@@ -594,17 +600,35 @@
     <t>Medium: Low contrast, odd coloring</t>
   </si>
   <si>
-    <t>Nr Cells(bioinformatician)</t>
-  </si>
-  <si>
-    <t>Nr Cells(biologist)</t>
+    <t>Nr Cells
+(bioinformatician)</t>
+  </si>
+  <si>
+    <t>Nr Cells
+(biologist) 1st round of manual mark-ups</t>
+  </si>
+  <si>
+    <t>Nr Cells
+(biologist) 2nd round of manual mark-ups</t>
+  </si>
+  <si>
+    <t>Nr Cells organwise
+(bioinformatician)</t>
+  </si>
+  <si>
+    <t>Nr Cells organwise
+(biologist) 1st round of manual mark-ups</t>
+  </si>
+  <si>
+    <t>Nr Cells organwise
+(biologist) 2nd round of manual mark-ups</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -658,6 +682,13 @@
       <u/>
       <sz val="10"/>
       <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -740,7 +771,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -762,10 +793,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -977,27 +1015,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:Y53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" topLeftCell="L4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2:U32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="43" customWidth="1"/>
     <col min="12" max="12" width="40" customWidth="1"/>
-    <col min="13" max="13" width="21.42578125" customWidth="1"/>
-    <col min="14" max="14" width="17.85546875" customWidth="1"/>
-    <col min="16" max="16" width="22.7109375" customWidth="1"/>
+    <col min="13" max="13" width="21.44140625" customWidth="1"/>
+    <col min="14" max="14" width="17.88671875" customWidth="1"/>
+    <col min="16" max="16" width="22.6640625" customWidth="1"/>
     <col min="17" max="17" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="12.75">
+    <row r="1" spans="1:25" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1043,17 +1081,29 @@
       <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="23" t="s">
         <v>187</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="Q1" s="23" t="s">
         <v>188</v>
       </c>
-      <c r="R1" s="18" t="s">
+      <c r="R1" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="S1" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="T1" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="U1" s="23" t="s">
+        <v>192</v>
+      </c>
+      <c r="V1" s="21" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="12.75">
+    <row r="2" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>105</v>
       </c>
@@ -1105,11 +1155,14 @@
       <c r="Q2" s="4">
         <v>85</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="R2" s="4">
+        <v>93</v>
+      </c>
+      <c r="V2" s="4" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="12.75">
+    <row r="3" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>110</v>
       </c>
@@ -1161,11 +1214,14 @@
       <c r="Q3">
         <v>119</v>
       </c>
-      <c r="R3" s="4" t="s">
+      <c r="R3">
+        <v>132</v>
+      </c>
+      <c r="V3" s="4" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="12.75">
+    <row r="4" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>113</v>
       </c>
@@ -1217,11 +1273,26 @@
       <c r="Q4">
         <v>134</v>
       </c>
-      <c r="R4" s="4" t="s">
+      <c r="R4">
+        <v>119</v>
+      </c>
+      <c r="S4">
+        <f>SUM(P2:P4)</f>
+        <v>392</v>
+      </c>
+      <c r="T4">
+        <f t="shared" ref="T4:U4" si="0">SUM(Q2:Q4)</f>
+        <v>338</v>
+      </c>
+      <c r="U4">
+        <f t="shared" si="0"/>
+        <v>344</v>
+      </c>
+      <c r="V4" s="4" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="12.75">
+    <row r="5" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>148</v>
       </c>
@@ -1273,11 +1344,14 @@
       <c r="Q5" s="4">
         <v>220</v>
       </c>
-      <c r="R5" s="4" t="s">
+      <c r="R5" s="4">
+        <v>227</v>
+      </c>
+      <c r="V5" s="4" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="12.75">
+    <row r="6" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>151</v>
       </c>
@@ -1329,17 +1403,18 @@
       <c r="Q6" s="4">
         <v>224</v>
       </c>
-      <c r="R6" s="4" t="s">
+      <c r="R6" s="4">
+        <v>223</v>
+      </c>
+      <c r="U6" s="9"/>
+      <c r="V6" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="T6" s="9"/>
-      <c r="U6" s="9"/>
-      <c r="V6" s="9"/>
       <c r="W6" s="9"/>
       <c r="X6" s="9"/>
       <c r="Y6" s="9"/>
     </row>
-    <row r="7" spans="1:25" ht="12.75">
+    <row r="7" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>154</v>
       </c>
@@ -1391,11 +1466,26 @@
       <c r="Q7" s="4">
         <v>178</v>
       </c>
-      <c r="R7" s="4" t="s">
+      <c r="R7" s="4">
+        <v>191</v>
+      </c>
+      <c r="S7">
+        <f>SUM(P5:P7)</f>
+        <v>765</v>
+      </c>
+      <c r="T7">
+        <f t="shared" ref="T7:U7" si="1">SUM(Q5:Q7)</f>
+        <v>622</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="1"/>
+        <v>641</v>
+      </c>
+      <c r="V7" s="4" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="12.75">
+    <row r="8" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>116</v>
       </c>
@@ -1447,11 +1537,14 @@
       <c r="Q8" s="4">
         <v>261</v>
       </c>
-      <c r="R8" s="4" t="s">
+      <c r="R8" s="4">
+        <v>292</v>
+      </c>
+      <c r="V8" s="4" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="12.75">
+    <row r="9" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>121</v>
       </c>
@@ -1503,11 +1596,14 @@
       <c r="Q9" s="4">
         <v>428</v>
       </c>
-      <c r="R9" s="4" t="s">
+      <c r="R9" s="4">
+        <v>449</v>
+      </c>
+      <c r="V9" s="4" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="12.75">
+    <row r="10" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>70</v>
       </c>
@@ -1559,11 +1655,26 @@
       <c r="Q10" s="4">
         <v>515</v>
       </c>
-      <c r="R10" s="4" t="s">
+      <c r="R10" s="4">
+        <v>567</v>
+      </c>
+      <c r="S10">
+        <f>SUM(P8:P10)</f>
+        <v>1353</v>
+      </c>
+      <c r="T10">
+        <f t="shared" ref="T10:U10" si="2">SUM(Q8:Q10)</f>
+        <v>1204</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="2"/>
+        <v>1308</v>
+      </c>
+      <c r="V10" s="4" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="12.75">
+    <row r="11" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>78</v>
       </c>
@@ -1615,11 +1726,14 @@
       <c r="Q11" s="4">
         <v>573</v>
       </c>
-      <c r="R11" s="4" t="s">
+      <c r="R11" s="4">
+        <v>598</v>
+      </c>
+      <c r="V11" s="4" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="12.75">
+    <row r="12" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>83</v>
       </c>
@@ -1671,12 +1785,15 @@
       <c r="Q12" s="4">
         <v>380</v>
       </c>
-      <c r="R12" s="4" t="s">
+      <c r="R12" s="4">
+        <v>411</v>
+      </c>
+      <c r="V12" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="T12" s="4"/>
-    </row>
-    <row r="13" spans="1:25" ht="12.75">
+      <c r="W12" s="4"/>
+    </row>
+    <row r="13" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>87</v>
       </c>
@@ -1728,11 +1845,26 @@
       <c r="Q13" s="4">
         <v>321</v>
       </c>
-      <c r="R13" s="4" t="s">
+      <c r="R13" s="4">
+        <v>340</v>
+      </c>
+      <c r="S13">
+        <f>SUM(P11:P13)</f>
+        <v>1354</v>
+      </c>
+      <c r="T13">
+        <f t="shared" ref="T13:U13" si="3">SUM(Q11:Q13)</f>
+        <v>1274</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="3"/>
+        <v>1349</v>
+      </c>
+      <c r="V13" s="4" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="12.75">
+    <row r="14" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>48</v>
       </c>
@@ -1784,11 +1916,14 @@
       <c r="Q14" s="4">
         <v>136</v>
       </c>
-      <c r="R14" s="4" t="s">
+      <c r="R14" s="4">
+        <v>188</v>
+      </c>
+      <c r="V14" s="4" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="12.75">
+    <row r="15" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>54</v>
       </c>
@@ -1840,11 +1975,14 @@
       <c r="Q15" s="4">
         <v>221</v>
       </c>
-      <c r="R15" s="4" t="s">
+      <c r="R15" s="4">
+        <v>228</v>
+      </c>
+      <c r="V15" s="4" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="12.75">
+    <row r="16" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>59</v>
       </c>
@@ -1896,11 +2034,26 @@
       <c r="Q16" s="4">
         <v>113</v>
       </c>
-      <c r="R16" s="4" t="s">
+      <c r="R16" s="4">
+        <v>132</v>
+      </c>
+      <c r="S16">
+        <f>SUM(P14:P16)</f>
+        <v>623</v>
+      </c>
+      <c r="T16">
+        <f t="shared" ref="T16:U16" si="4">SUM(Q14:Q16)</f>
+        <v>470</v>
+      </c>
+      <c r="U16">
+        <f t="shared" si="4"/>
+        <v>548</v>
+      </c>
+      <c r="V16" s="4" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="12.75">
+    <row r="17" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>63</v>
       </c>
@@ -1952,11 +2105,14 @@
       <c r="Q17" s="4">
         <v>168</v>
       </c>
-      <c r="R17" s="4" t="s">
+      <c r="R17" s="4">
+        <v>168</v>
+      </c>
+      <c r="V17" s="4" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="12.75">
+    <row r="18" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>68</v>
       </c>
@@ -2008,11 +2164,14 @@
       <c r="Q18" s="4">
         <v>177</v>
       </c>
-      <c r="R18" s="4" t="s">
+      <c r="R18" s="4">
+        <v>199</v>
+      </c>
+      <c r="V18" s="4" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="12.75">
+    <row r="19" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>73</v>
       </c>
@@ -2064,11 +2223,26 @@
       <c r="Q19" s="4">
         <v>152</v>
       </c>
-      <c r="R19" s="4" t="s">
+      <c r="R19" s="4">
+        <v>148</v>
+      </c>
+      <c r="S19">
+        <f>SUM(P17:P19)</f>
+        <v>638</v>
+      </c>
+      <c r="T19">
+        <f t="shared" ref="T19:U19" si="5">SUM(Q17:Q19)</f>
+        <v>497</v>
+      </c>
+      <c r="U19">
+        <f t="shared" si="5"/>
+        <v>515</v>
+      </c>
+      <c r="V19" s="4" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="15.75" customHeight="1">
+    <row r="20" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>34</v>
       </c>
@@ -2120,11 +2294,14 @@
       <c r="Q20" s="4">
         <v>144</v>
       </c>
-      <c r="R20" s="4" t="s">
+      <c r="R20" s="4">
+        <v>137</v>
+      </c>
+      <c r="V20" s="4" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="15.75" customHeight="1">
+    <row r="21" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>39</v>
       </c>
@@ -2176,11 +2353,14 @@
       <c r="Q21" s="4">
         <v>126</v>
       </c>
-      <c r="R21" s="4" t="s">
+      <c r="R21" s="4">
+        <v>126</v>
+      </c>
+      <c r="V21" s="4" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="15.75" customHeight="1">
+    <row r="22" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>44</v>
       </c>
@@ -2232,11 +2412,26 @@
       <c r="Q22" s="4">
         <v>187</v>
       </c>
-      <c r="R22" s="4" t="s">
+      <c r="R22" s="4">
+        <v>173</v>
+      </c>
+      <c r="S22">
+        <f>SUM(P20:P22)</f>
+        <v>507</v>
+      </c>
+      <c r="T22">
+        <f t="shared" ref="T22:U22" si="6">SUM(Q20:Q22)</f>
+        <v>457</v>
+      </c>
+      <c r="U22">
+        <f t="shared" si="6"/>
+        <v>436</v>
+      </c>
+      <c r="V22" s="4" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="12.75">
+    <row r="23" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>139</v>
       </c>
@@ -2279,11 +2474,14 @@
       <c r="Q23" s="4">
         <v>274</v>
       </c>
-      <c r="R23" s="4" t="s">
+      <c r="R23" s="4">
+        <v>277</v>
+      </c>
+      <c r="V23" s="4" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="12.75">
+    <row r="24" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
         <v>140</v>
       </c>
@@ -2335,11 +2533,14 @@
       <c r="Q24" s="4">
         <v>249</v>
       </c>
-      <c r="R24" s="4" t="s">
+      <c r="R24" s="4">
+        <v>268</v>
+      </c>
+      <c r="V24" s="4" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="12.75">
+    <row r="25" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>141</v>
       </c>
@@ -2391,11 +2592,26 @@
       <c r="Q25" s="4">
         <v>229</v>
       </c>
-      <c r="R25" s="4" t="s">
+      <c r="R25" s="4">
+        <v>248</v>
+      </c>
+      <c r="S25">
+        <f>SUM(P23:P25)</f>
+        <v>687</v>
+      </c>
+      <c r="T25">
+        <f t="shared" ref="T25:U25" si="7">SUM(Q23:Q25)</f>
+        <v>752</v>
+      </c>
+      <c r="U25">
+        <f t="shared" si="7"/>
+        <v>793</v>
+      </c>
+      <c r="V25" s="4" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="12.75">
+    <row r="26" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>91</v>
       </c>
@@ -2447,11 +2663,14 @@
       <c r="Q26" s="4">
         <v>638</v>
       </c>
-      <c r="R26" s="4" t="s">
+      <c r="R26" s="4">
+        <v>666</v>
+      </c>
+      <c r="V26" s="4" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="12.75">
+    <row r="27" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>96</v>
       </c>
@@ -2503,11 +2722,14 @@
       <c r="Q27" s="4">
         <v>597</v>
       </c>
-      <c r="R27" s="4" t="s">
+      <c r="R27" s="4">
+        <v>659</v>
+      </c>
+      <c r="V27" s="4" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="12.75">
+    <row r="28" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>101</v>
       </c>
@@ -2559,11 +2781,26 @@
       <c r="Q28" s="4">
         <v>286</v>
       </c>
-      <c r="R28" s="4" t="s">
+      <c r="R28" s="4">
+        <v>321</v>
+      </c>
+      <c r="S28">
+        <f>SUM(P26:P28)</f>
+        <v>1483</v>
+      </c>
+      <c r="T28">
+        <f t="shared" ref="T28:U28" si="8">SUM(Q26:Q28)</f>
+        <v>1521</v>
+      </c>
+      <c r="U28">
+        <f t="shared" si="8"/>
+        <v>1646</v>
+      </c>
+      <c r="V28" s="4" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="15.75" customHeight="1">
+    <row r="29" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>15</v>
       </c>
@@ -2615,11 +2852,14 @@
       <c r="Q29" s="4">
         <v>117</v>
       </c>
-      <c r="R29" s="4" t="s">
+      <c r="R29" s="4">
+        <v>128</v>
+      </c>
+      <c r="V29" s="4" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="15.75" customHeight="1">
+    <row r="30" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>26</v>
       </c>
@@ -2671,11 +2911,14 @@
       <c r="Q30" s="4">
         <v>158</v>
       </c>
-      <c r="R30" s="4" t="s">
+      <c r="R30" s="4">
+        <v>149</v>
+      </c>
+      <c r="V30" s="4" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="31" spans="1:18" ht="15.75" customHeight="1">
+    <row r="31" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>31</v>
       </c>
@@ -2727,11 +2970,26 @@
       <c r="Q31" s="4">
         <v>186</v>
       </c>
-      <c r="R31" s="4" t="s">
+      <c r="R31" s="4">
+        <v>187</v>
+      </c>
+      <c r="S31">
+        <f>SUM(P29:P31)</f>
+        <v>449</v>
+      </c>
+      <c r="T31">
+        <f t="shared" ref="T31:U31" si="9">SUM(Q29:Q31)</f>
+        <v>461</v>
+      </c>
+      <c r="U31">
+        <f t="shared" si="9"/>
+        <v>464</v>
+      </c>
+      <c r="V31" s="4" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="15.75" customHeight="1">
+    <row r="32" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="P32">
         <f>SUM(P2:P31)</f>
         <v>8251</v>
@@ -2740,13 +2998,32 @@
         <f>SUM(Q2:Q31)</f>
         <v>7596</v>
       </c>
-    </row>
-    <row r="50" spans="7:10" ht="12.75">
+      <c r="R32">
+        <f>SUM(R2:R31)</f>
+        <v>8044</v>
+      </c>
+      <c r="S32">
+        <f>SUM(S2:S31)</f>
+        <v>8251</v>
+      </c>
+      <c r="T32">
+        <f t="shared" ref="T32:U32" si="10">SUM(T2:T31)</f>
+        <v>7596</v>
+      </c>
+      <c r="U32">
+        <f t="shared" si="10"/>
+        <v>8044</v>
+      </c>
+    </row>
+    <row r="36" spans="21:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U36" s="22"/>
+    </row>
+    <row r="50" spans="7:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G50" s="4" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="52" spans="7:10" ht="12.75">
+    <row r="52" spans="7:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G52" s="6" t="s">
         <v>127</v>
       </c>
@@ -2760,7 +3037,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="53" spans="7:10" ht="12.75">
+    <row r="53" spans="7:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G53" s="8" t="s">
         <v>130</v>
       </c>
@@ -2772,40 +3049,40 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:Q31">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q31">
     <sortCondition ref="M2:M31"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="A29" r:id="rId1"/>
-    <hyperlink ref="A30" r:id="rId2"/>
-    <hyperlink ref="A31" r:id="rId3"/>
-    <hyperlink ref="A20" r:id="rId4"/>
-    <hyperlink ref="A21" r:id="rId5"/>
-    <hyperlink ref="A22" r:id="rId6"/>
-    <hyperlink ref="A14" r:id="rId7"/>
-    <hyperlink ref="A15" r:id="rId8"/>
-    <hyperlink ref="A16" r:id="rId9"/>
-    <hyperlink ref="A17" r:id="rId10"/>
-    <hyperlink ref="A18" r:id="rId11"/>
-    <hyperlink ref="A19" r:id="rId12"/>
-    <hyperlink ref="A11" r:id="rId13"/>
-    <hyperlink ref="A12" r:id="rId14"/>
-    <hyperlink ref="A13" r:id="rId15"/>
-    <hyperlink ref="A26" r:id="rId16"/>
-    <hyperlink ref="A27" r:id="rId17"/>
-    <hyperlink ref="A28" r:id="rId18"/>
-    <hyperlink ref="A2" r:id="rId19"/>
-    <hyperlink ref="A3" r:id="rId20"/>
-    <hyperlink ref="A4" r:id="rId21"/>
-    <hyperlink ref="A8" r:id="rId22"/>
-    <hyperlink ref="A9" r:id="rId23"/>
-    <hyperlink ref="A10" r:id="rId24"/>
-    <hyperlink ref="A23" r:id="rId25"/>
-    <hyperlink ref="A5" r:id="rId26"/>
-    <hyperlink ref="A6" r:id="rId27"/>
-    <hyperlink ref="A7" r:id="rId28"/>
-    <hyperlink ref="A24" r:id="rId29"/>
-    <hyperlink ref="A25" r:id="rId30"/>
+    <hyperlink ref="A29" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A30" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A31" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="A20" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="A21" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="A22" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="A14" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="A15" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="A16" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="A17" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="A18" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="A19" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="A11" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="A12" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="A13" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="A26" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="A27" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="A28" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="A2" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="A3" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="A4" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="A8" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="A9" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="A10" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="A23" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="A5" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="A6" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="A7" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="A24" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="A25" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId31"/>

</xml_diff>